<commit_message>
feat(MorningSun): Import policy, open to all company
</commit_message>
<xml_diff>
--- a/AccuPay/ImportTemplates/accupay-govt-premium-template.xlsx
+++ b/AccuPay/ImportTemplates/accupay-govt-premium-template.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>Employee ID</t>
   </si>
@@ -56,6 +56,9 @@
   </si>
   <si>
     <t>HDMF Employer Share</t>
+  </si>
+  <si>
+    <t>EmployeeRowId</t>
   </si>
 </sst>
 </file>
@@ -91,7 +94,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -140,11 +143,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyProtection="1">
       <protection locked="0"/>
@@ -159,6 +173,9 @@
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -436,7 +453,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J2"/>
+  <dimension ref="A1:K2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -445,7 +462,7 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="25" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="89.7109375" style="1" customWidth="1"/>
     <col min="2" max="2" width="19" style="3" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="18.5703125" style="3" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="21.140625" style="3" bestFit="1" customWidth="1"/>
@@ -455,10 +472,11 @@
     <col min="8" max="8" width="25" style="3"/>
     <col min="9" max="9" width="21.5703125" style="3" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="21" style="3" bestFit="1" customWidth="1"/>
-    <col min="11" max="16384" width="25" style="5"/>
+    <col min="11" max="11" width="0" style="5" hidden="1" customWidth="1"/>
+    <col min="12" max="16384" width="25" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -489,12 +507,15 @@
       <c r="J1" s="7" t="s">
         <v>11</v>
       </c>
+      <c r="K1" s="8" t="s">
+        <v>12</v>
+      </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="6"/>
     </row>
   </sheetData>
-  <sheetProtection sheet="1" objects="1" scenarios="1" insertRows="0" deleteRows="0"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="D7q+QoY9tYtSaQ66BQHugM//g161Y2oupf/YZCfsAq1UJ6Y2zu7gupxx7evW5W6sn3TIgCWzCD7hkHG5bTt2cA==" saltValue="M01BkvXemyGOh8GS5e+N+Q==" spinCount="100000" sheet="1" objects="1" scenarios="1" insertRows="0" deleteRows="0" selectLockedCells="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
fix: government premium import open to all method
</commit_message>
<xml_diff>
--- a/AccuPay/ImportTemplates/accupay-govt-premium-template.xlsx
+++ b/AccuPay/ImportTemplates/accupay-govt-premium-template.xlsx
@@ -86,12 +86,30 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="5">
@@ -158,7 +176,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyProtection="1">
       <protection locked="0"/>
@@ -167,17 +185,21 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1"/>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -472,27 +494,27 @@
     <col min="8" max="8" width="25" style="3"/>
     <col min="9" max="9" width="21.5703125" style="3" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="21" style="3" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="0" style="5" hidden="1" customWidth="1"/>
-    <col min="12" max="16384" width="25" style="5"/>
+    <col min="11" max="11" width="0" style="4" hidden="1" customWidth="1"/>
+    <col min="12" max="16384" width="25" style="4"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="F1" s="10" t="s">
         <v>7</v>
       </c>
       <c r="G1" s="7" t="s">
@@ -501,21 +523,21 @@
       <c r="H1" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="I1" s="7" t="s">
+      <c r="I1" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="J1" s="7" t="s">
+      <c r="J1" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="K1" s="8" t="s">
+      <c r="K1" s="6" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" s="6"/>
+      <c r="A2" s="5"/>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="D7q+QoY9tYtSaQ66BQHugM//g161Y2oupf/YZCfsAq1UJ6Y2zu7gupxx7evW5W6sn3TIgCWzCD7hkHG5bTt2cA==" saltValue="M01BkvXemyGOh8GS5e+N+Q==" spinCount="100000" sheet="1" objects="1" scenarios="1" insertRows="0" deleteRows="0" selectLockedCells="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="J2RKWVxJ7XUBQKxc/hBbLozSvvaEyidKqM6C0TlNImCVpJy1ic5XKZOnpDjuQHocHufw6XctLOZeLR8/eYkj0w==" saltValue="g1F7t5BxT4Qa3o4XItZn1A==" spinCount="100000" sheet="1" objects="1" scenarios="1" insertRows="0" deleteRows="0" selectLockedCells="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>